<commit_message>
Devices types and metrics by building scripts
</commit_message>
<xml_diff>
--- a/PrimeCore.xlsx
+++ b/PrimeCore.xlsx
@@ -10759,7 +10759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G793"/>
+  <dimension ref="A1:G795"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A773" xSplit="0" ySplit="1"/>
@@ -32066,22 +32066,62 @@
       </c>
     </row>
     <row r="793">
-      <c r="A793" t="n">
+      <c r="A793" s="32" t="n">
         <v>8865742261</v>
       </c>
-      <c r="B793" t="inlineStr">
-        <is>
-          <t>default location</t>
-        </is>
-      </c>
-      <c r="C793" t="inlineStr">
+      <c r="B793" s="32" t="inlineStr">
+        <is>
+          <t>default location</t>
+        </is>
+      </c>
+      <c r="C793" s="32" t="inlineStr">
         <is>
           <t>essua-ap66</t>
         </is>
       </c>
-      <c r="G793" t="inlineStr">
+      <c r="G793" s="32" t="inlineStr">
         <is>
           <t>essua</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" s="32" t="n">
+        <v>8865742280</v>
+      </c>
+      <c r="B794" s="32" t="inlineStr">
+        <is>
+          <t>default location</t>
+        </is>
+      </c>
+      <c r="C794" s="32" t="inlineStr">
+        <is>
+          <t>demac-ap16</t>
+        </is>
+      </c>
+      <c r="G794" s="32" t="inlineStr">
+        <is>
+          <t>demac</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="n">
+        <v>8865742282</v>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>default location</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>ra-b10-ap02-new</t>
+        </is>
+      </c>
+      <c r="G795" t="inlineStr">
+        <is>
+          <t>ra</t>
         </is>
       </c>
     </row>

</xml_diff>